<commit_message>
Added support for PO # rules. Refactoring.
</commit_message>
<xml_diff>
--- a/Escalator/Rules.xlsx
+++ b/Escalator/Rules.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Mike\Repos\escalator\Escalator\bin\Debug\net5.0-windows\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Mike\Repos\escalator\Escalator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{968CFE12-2B59-47B7-A12C-E5C736FF6B2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E11013D-D6E6-4475-A57D-0051DAD812D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3285" yWindow="3285" windowWidth="21600" windowHeight="11325" xr2:uid="{11098DB5-0275-4CDE-ACC3-5D76E0E97528}"/>
+    <workbookView xWindow="3990" yWindow="1020" windowWidth="21600" windowHeight="11325" xr2:uid="{11098DB5-0275-4CDE-ACC3-5D76E0E97528}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Company</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>Address</t>
+  </si>
+  <si>
+    <t>Use PO#</t>
   </si>
 </sst>
 </file>
@@ -417,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59830DB2-BA7E-44B4-BBCA-6609E2497F05}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="B2:F2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,7 +436,7 @@
     <col min="7" max="7" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -455,11 +458,14 @@
       <c r="G1" t="s">
         <v>4</v>
       </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E3" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Integrated both rulesets into the same excel sheet, as well as the previous .settings items. Spot lot is now a read-only property. Added support for rule search by email and rule updates to subdivisions.
</commit_message>
<xml_diff>
--- a/Escalator/Rules.xlsx
+++ b/Escalator/Rules.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Mike\Repos\escalator\Escalator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E11013D-D6E6-4475-A57D-0051DAD812D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A79753C-51AE-4BE6-9410-09ED6FD51F83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3990" yWindow="1020" windowWidth="21600" windowHeight="11325" xr2:uid="{11098DB5-0275-4CDE-ACC3-5D76E0E97528}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Order Import Rules" sheetId="1" r:id="rId1"/>
+    <sheet name="Subdivision Word Replacements" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
   <si>
     <t>Company</t>
   </si>
@@ -45,26 +46,167 @@
     <t>Lot</t>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Show Error</t>
-  </si>
-  <si>
-    <t>Skip Combination</t>
-  </si>
-  <si>
     <t>Address</t>
   </si>
   <si>
     <t>Use PO#</t>
+  </si>
+  <si>
+    <t>Rules to Apply</t>
+  </si>
+  <si>
+    <t>Order Search Criteria</t>
+  </si>
+  <si>
+    <t>Updated Email</t>
+  </si>
+  <si>
+    <t>Original Email</t>
+  </si>
+  <si>
+    <t>Show Warning</t>
+  </si>
+  <si>
+    <t>Raw Import</t>
+  </si>
+  <si>
+    <t>Updated Subdivision</t>
+  </si>
+  <si>
+    <t>Word</t>
+  </si>
+  <si>
+    <t>Replace With</t>
+  </si>
+  <si>
+    <t>To</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>At</t>
+  </si>
+  <si>
+    <t>at</t>
+  </si>
+  <si>
+    <t>In</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>Of</t>
+  </si>
+  <si>
+    <t>of</t>
+  </si>
+  <si>
+    <t>The</t>
+  </si>
+  <si>
+    <t>the</t>
+  </si>
+  <si>
+    <t>By</t>
+  </si>
+  <si>
+    <t>by</t>
+  </si>
+  <si>
+    <t>For</t>
+  </si>
+  <si>
+    <t>for</t>
+  </si>
+  <si>
+    <t>Ii</t>
+  </si>
+  <si>
+    <t>II</t>
+  </si>
+  <si>
+    <t>Iii</t>
+  </si>
+  <si>
+    <t>III</t>
+  </si>
+  <si>
+    <t>Iv</t>
+  </si>
+  <si>
+    <t>IV</t>
+  </si>
+  <si>
+    <t>Vi</t>
+  </si>
+  <si>
+    <t>VI</t>
+  </si>
+  <si>
+    <t>Viii</t>
+  </si>
+  <si>
+    <t>VIII</t>
+  </si>
+  <si>
+    <t>Ix</t>
+  </si>
+  <si>
+    <t>IX</t>
+  </si>
+  <si>
+    <t>Xi</t>
+  </si>
+  <si>
+    <t>XI</t>
+  </si>
+  <si>
+    <t>Xii</t>
+  </si>
+  <si>
+    <t>XII</t>
+  </si>
+  <si>
+    <t>Xiii</t>
+  </si>
+  <si>
+    <t>XIII</t>
+  </si>
+  <si>
+    <t>Xiv</t>
+  </si>
+  <si>
+    <t>XIV</t>
+  </si>
+  <si>
+    <t>Xv</t>
+  </si>
+  <si>
+    <t>XV</t>
+  </si>
+  <si>
+    <t>Th</t>
+  </si>
+  <si>
+    <t>TH</t>
+  </si>
+  <si>
+    <t>SPOT LOT</t>
+  </si>
+  <si>
+    <t>SPOPT LOT</t>
+  </si>
+  <si>
+    <t>#blank</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,16 +222,44 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -97,14 +267,58 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -420,10 +634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59830DB2-BA7E-44B4-BBCA-6609E2497F05}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,44 +645,267 @@
     <col min="1" max="1" width="15.85546875" customWidth="1"/>
     <col min="2" max="2" width="23.42578125" customWidth="1"/>
     <col min="3" max="4" width="14.5703125" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" customWidth="1"/>
-    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="E2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E3" s="1"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE8EA96C-6EA6-4CDD-B55D-5989A72D6F89}">
+  <dimension ref="A1:B22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" t="s">
+        <v>51</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed rule import. Auto-select of stairs vs rails now done based on filename. Added text "PO" to all PO verify list records.
</commit_message>
<xml_diff>
--- a/Escalator/Rules.xlsx
+++ b/Escalator/Rules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Mike\Repos\escalator\Escalator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A79753C-51AE-4BE6-9410-09ED6FD51F83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7C03604-7E0C-4FE1-80EF-EB9D96506AFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3990" yWindow="1020" windowWidth="21600" windowHeight="11325" xr2:uid="{11098DB5-0275-4CDE-ACC3-5D76E0E97528}"/>
+    <workbookView xWindow="2115" yWindow="1530" windowWidth="22815" windowHeight="11505" xr2:uid="{11098DB5-0275-4CDE-ACC3-5D76E0E97528}"/>
   </bookViews>
   <sheets>
     <sheet name="Order Import Rules" sheetId="1" r:id="rId1"/>
@@ -301,23 +301,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -637,85 +650,86 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" customWidth="1"/>
-    <col min="3" max="4" width="14.5703125" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" customWidth="1"/>
+    <col min="1" max="1" width="35.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="34.7109375" style="3" customWidth="1"/>
+    <col min="3" max="4" width="14.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28" style="3" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="8" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="G3" t="s">
+      <c r="F3" s="8"/>
+      <c r="G3" s="3" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="F4" s="1"/>
-      <c r="G4" t="s">
+      <c r="F4" s="8"/>
+      <c r="G4" s="3" t="s">
         <v>54</v>
       </c>
     </row>
@@ -744,11 +758,11 @@
     <col min="3" max="3" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="2" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>